<commit_message>
yellow background color for low values
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhihuitang/repo/python/Provsvar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE93D4BC-5B3D-CC47-BB72-D3423FB6AE82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D62EDA-B549-6742-8812-D0E482417C35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="680" windowWidth="28040" windowHeight="17440" xr2:uid="{DBE3080E-B9F2-3742-A561-42170D0095D6}"/>
   </bookViews>
@@ -505,7 +505,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -747,10 +747,22 @@
       <c r="A23" t="s">
         <v>18</v>
       </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>19</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>